<commit_message>
Volume PMS Fixes #36
</commit_message>
<xml_diff>
--- a/data-raw/resenhas/legenda-conjuntura.xlsx
+++ b/data-raw/resenhas/legenda-conjuntura.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>pib</t>
   </si>
@@ -35,9 +35,6 @@
     <t>ibc.br</t>
   </si>
   <si>
-    <t>varejo.servico</t>
-  </si>
-  <si>
     <t>exportacoes</t>
   </si>
   <si>
@@ -156,6 +153,12 @@
   </si>
   <si>
     <t>Neste caso, o resultado primário negativo significa superávit, enquando o positivo significa déficit.</t>
+  </si>
+  <si>
+    <t>servicos</t>
+  </si>
+  <si>
+    <t>varejo</t>
   </si>
 </sst>
 </file>
@@ -493,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,32 +508,33 @@
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" customWidth="1"/>
-    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.7109375" customWidth="1"/>
-    <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.42578125" customWidth="1"/>
-    <col min="28" max="28" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" customWidth="1"/>
+    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.7109375" customWidth="1"/>
+    <col min="27" max="27" width="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.42578125" customWidth="1"/>
+    <col min="29" max="29" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,110 +545,113 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:33" ht="329.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" ht="329.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -655,32 +662,33 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
-      <c r="S2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
-      <c r="X2" s="4" t="s">
+      <c r="W2" s="2"/>
+      <c r="Y2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="Z2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="AF2" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Colocando legenda correta nas boxes de "Indústria".
</commit_message>
<xml_diff>
--- a/data-raw/resenhas/legenda-conjuntura.xlsx
+++ b/data-raw/resenhas/legenda-conjuntura.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>pib</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>Neste caso, o resultado primário negativo significa superávit, enquando o positivo significa déficit.</t>
+  </si>
+  <si>
+    <t>industria</t>
+  </si>
+  <si>
+    <t>industria.es</t>
   </si>
 </sst>
 </file>
@@ -493,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,32 +511,34 @@
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" customWidth="1"/>
-    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.7109375" customWidth="1"/>
-    <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.42578125" customWidth="1"/>
-    <col min="28" max="28" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" customWidth="1"/>
+    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.7109375" customWidth="1"/>
+    <col min="28" max="28" width="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.42578125" customWidth="1"/>
+    <col min="30" max="30" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,91 +552,97 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="329.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="329.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
@@ -638,13 +652,13 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -655,31 +669,33 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
       <c r="V2" s="2"/>
-      <c r="X2" s="4" t="s">
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Z2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AF2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de legenda dos gráficos.
</commit_message>
<xml_diff>
--- a/data-raw/resenhas/legenda-conjuntura.xlsx
+++ b/data-raw/resenhas/legenda-conjuntura.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>pib</t>
   </si>
@@ -35,9 +35,6 @@
     <t>ibc.br</t>
   </si>
   <si>
-    <t>varejo.servico</t>
-  </si>
-  <si>
     <t>exportacoes</t>
   </si>
   <si>
@@ -162,13 +159,19 @@
   </si>
   <si>
     <t>industria.es</t>
+  </si>
+  <si>
+    <t>servicos</t>
+  </si>
+  <si>
+    <t>varejo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +181,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -205,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -218,6 +229,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -499,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,34 +525,34 @@
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.7109375" customWidth="1"/>
-    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.7109375" customWidth="1"/>
-    <col min="28" max="28" width="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.42578125" customWidth="1"/>
-    <col min="30" max="30" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" customWidth="1"/>
+    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.7109375" customWidth="1"/>
+    <col min="29" max="29" width="11" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.42578125" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,117 +563,120 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:35" ht="329.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:34" ht="329.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="E2" s="5"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -671,32 +688,33 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="U2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="V2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
-      <c r="Z2" s="4" t="s">
+      <c r="Y2" s="2"/>
+      <c r="AA2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AB2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AF2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="AH2" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>